<commit_message>
opt@brand#:add permission control config.
</commit_message>
<xml_diff>
--- a/VersionRecords/Version Brand/BS权限/新增--修改--删除--权限配置表.xlsx
+++ b/VersionRecords/Version Brand/BS权限/新增--修改--删除--权限配置表.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\Mogo_Doc\VersionRecords\Version Brand\BS权限\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2775" windowWidth="27540" windowHeight="10635"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="126">
   <si>
     <t>级别</t>
   </si>
@@ -804,12 +809,28 @@
     <t>顶部轮播广告位管理</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>编辑器上传文件</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>品牌管理-优先品牌管理-品牌评测管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>品牌管理-优先品牌管理-品牌评测管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cms/addContextForUploadPic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1083,7 +1104,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1115,9 +1136,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1149,6 +1171,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1324,14 +1347,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="64.625" customWidth="1"/>
     <col min="3" max="3" width="42.125" customWidth="1"/>
@@ -1339,7 +1362,7 @@
     <col min="9" max="9" width="24.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1368,7 +1391,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>3</v>
       </c>
@@ -1395,7 +1418,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>3</v>
       </c>
@@ -1422,13 +1445,13 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B4" s="5"/>
       <c r="D4" s="5"/>
       <c r="F4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1439,7 +1462,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="3"/>
@@ -1450,7 +1473,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="3"/>
@@ -1461,13 +1484,13 @@
       <c r="H7" s="4"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B8" s="5"/>
       <c r="D8" s="5"/>
       <c r="F8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1478,7 +1501,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>3</v>
       </c>
@@ -1503,7 +1526,7 @@
       </c>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>4</v>
       </c>
@@ -1530,7 +1553,7 @@
       </c>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1556,12 +1579,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>4</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>112</v>
@@ -1582,18 +1605,34 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="4"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="3"/>
@@ -1604,14 +1643,14 @@
       <c r="H15" s="4"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B16" s="5"/>
       <c r="C16" s="3"/>
       <c r="D16" s="4"/>
       <c r="F16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="D17" s="5"/>
@@ -1621,7 +1660,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="3"/>
@@ -1632,7 +1671,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3"/>
@@ -1643,20 +1682,20 @@
       <c r="H19" s="4"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B20" s="5"/>
       <c r="C20" s="3"/>
       <c r="D20" s="4"/>
       <c r="F20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B21" s="5"/>
       <c r="D21" s="5"/>
       <c r="F21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="5"/>
       <c r="D22" s="3"/>
@@ -1666,7 +1705,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
@@ -1685,14 +1724,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="56.875" customWidth="1"/>
     <col min="3" max="3" width="31.375" customWidth="1"/>
@@ -1701,7 +1740,7 @@
     <col min="10" max="10" width="24.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="14.25" thickBot="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1733,7 +1772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>3</v>
       </c>
@@ -1759,7 +1798,7 @@
       </c>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>3</v>
       </c>
@@ -1785,7 +1824,7 @@
       </c>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1811,7 +1850,7 @@
       </c>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1837,7 +1876,7 @@
       </c>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -1863,7 +1902,7 @@
       </c>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -1889,7 +1928,7 @@
       </c>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>3</v>
       </c>
@@ -1915,7 +1954,7 @@
       </c>
       <c r="J8" s="13"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>3</v>
       </c>
@@ -1941,7 +1980,7 @@
       </c>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>3</v>
       </c>
@@ -1967,7 +2006,7 @@
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="14"/>
       <c r="C11" s="3"/>
@@ -1979,7 +2018,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="3"/>
@@ -1991,7 +2030,7 @@
       <c r="I12" s="7"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="3"/>
@@ -2003,7 +2042,7 @@
       <c r="I13" s="7"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
@@ -2015,7 +2054,7 @@
       <c r="I14" s="7"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
@@ -2027,7 +2066,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="7"/>
       <c r="B16" s="4"/>
       <c r="C16" s="8"/>
@@ -2039,7 +2078,7 @@
       <c r="I16" s="7"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="7"/>
       <c r="B17" s="4"/>
       <c r="C17" s="7"/>
@@ -2051,7 +2090,7 @@
       <c r="I17" s="7"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -2063,7 +2102,7 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3"/>
@@ -2075,7 +2114,7 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="7"/>
       <c r="C20" s="3"/>
@@ -2087,7 +2126,7 @@
       <c r="I20" s="7"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -2099,7 +2138,7 @@
       <c r="I21" s="4"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="8"/>
       <c r="C22" s="7"/>
@@ -2111,7 +2150,7 @@
       <c r="I22" s="7"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="3"/>
@@ -2123,7 +2162,7 @@
       <c r="I23" s="7"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="8"/>
       <c r="C24" s="7"/>
@@ -2135,7 +2174,7 @@
       <c r="I24" s="7"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" ht="14.25" thickBot="1">
+    <row r="25" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="10"/>
       <c r="C25" s="11"/>
@@ -2155,14 +2194,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="43.5" customWidth="1"/>
     <col min="3" max="3" width="43.625" customWidth="1"/>
@@ -2172,7 +2211,7 @@
     <col min="9" max="9" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.25" thickBot="1">
+    <row r="1" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2201,7 +2240,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>3</v>
       </c>
@@ -2224,7 +2263,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>3</v>
       </c>
@@ -2247,7 +2286,7 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2270,7 +2309,7 @@
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -2293,7 +2332,7 @@
       </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -2316,7 +2355,7 @@
       </c>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -2339,7 +2378,7 @@
       </c>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>3</v>
       </c>
@@ -2362,7 +2401,7 @@
       </c>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>3</v>
       </c>
@@ -2385,7 +2424,7 @@
       </c>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>3</v>
       </c>
@@ -2408,7 +2447,7 @@
       </c>
       <c r="I10" s="8"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>3</v>
       </c>
@@ -2431,7 +2470,7 @@
       </c>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>3</v>
       </c>
@@ -2454,7 +2493,7 @@
       </c>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>3</v>
       </c>
@@ -2477,7 +2516,7 @@
       </c>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>3</v>
       </c>
@@ -2500,7 +2539,7 @@
       </c>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>3</v>
       </c>
@@ -2523,7 +2562,7 @@
       </c>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>3</v>
       </c>
@@ -2546,7 +2585,7 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>3</v>
       </c>
@@ -2569,7 +2608,7 @@
       </c>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>3</v>
       </c>
@@ -2592,7 +2631,7 @@
       </c>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>3</v>
       </c>
@@ -2615,7 +2654,7 @@
       </c>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>3</v>
       </c>
@@ -2638,7 +2677,7 @@
       </c>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>3</v>
       </c>
@@ -2661,7 +2700,7 @@
       </c>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>3</v>
       </c>
@@ -2684,7 +2723,7 @@
       </c>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>3</v>
       </c>
@@ -2707,7 +2746,7 @@
       </c>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>3</v>
       </c>
@@ -2730,7 +2769,7 @@
       </c>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>3</v>
       </c>
@@ -2753,7 +2792,7 @@
       </c>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>3</v>
       </c>
@@ -2776,7 +2815,7 @@
       </c>
       <c r="I26" s="21"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>3</v>
       </c>
@@ -2799,7 +2838,7 @@
       </c>
       <c r="I27" s="21"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -2810,7 +2849,7 @@
       <c r="H28" s="20"/>
       <c r="I28" s="21"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -2821,7 +2860,7 @@
       <c r="H29" s="20"/>
       <c r="I29" s="21"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -2832,7 +2871,7 @@
       <c r="H30" s="20"/>
       <c r="I30" s="21"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
@@ -2843,7 +2882,7 @@
       <c r="H31" s="20"/>
       <c r="I31" s="21"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -2854,7 +2893,7 @@
       <c r="H32" s="20"/>
       <c r="I32" s="21"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -2865,7 +2904,7 @@
       <c r="H33" s="20"/>
       <c r="I33" s="21"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -2876,7 +2915,7 @@
       <c r="H34" s="20"/>
       <c r="I34" s="21"/>
     </row>
-    <row r="35" spans="1:9" ht="14.25" thickBot="1">
+    <row r="35" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>

</xml_diff>